<commit_message>
modifi ids de juegos y retos en excel
pendiente tratamiento del array para filtrarlo por unidad clicqueada
</commit_message>
<xml_diff>
--- a/_DOCs/webserviseV2-0.xlsx
+++ b/_DOCs/webserviseV2-0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Confe2\_DOCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DAF958-164B-4999-8113-3B7D22A41694}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AA6AC2-0547-4C65-85E7-B3897E0E319B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13764" windowHeight="8040" xr2:uid="{92E7474C-DBF9-422C-8A46-30790FC12D63}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13764" windowHeight="8040" activeTab="2" xr2:uid="{92E7474C-DBF9-422C-8A46-30790FC12D63}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos WS" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="103">
   <si>
     <t>-</t>
   </si>
@@ -326,6 +326,21 @@
   </si>
   <si>
     <t>Se debe contar con un perfil de super usuario que tenga acceso a las anteriores funcionalidades de manera global (no por grupo) . A parte de un módulo para hacer un CRUD de textos por juego</t>
+  </si>
+  <si>
+    <t>r01emociones</t>
+  </si>
+  <si>
+    <t>c01ropero1</t>
+  </si>
+  <si>
+    <t>j01granja</t>
+  </si>
+  <si>
+    <t>c02ropero2</t>
+  </si>
+  <si>
+    <t>j02top10</t>
   </si>
 </sst>
 </file>
@@ -885,7 +900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081A2071-6B82-4DF7-B58A-E6A87EDE448E}">
   <dimension ref="B5:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -1186,14 +1201,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0627DF3-34FF-401C-8C73-99D44018DFCD}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="12"/>
-    <col min="2" max="2" width="9" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="11" customWidth="1"/>
     <col min="3" max="3" width="38.21875" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.109375" style="12" customWidth="1"/>
     <col min="5" max="6" width="8.88671875" style="13"/>
@@ -1236,6 +1251,9 @@
       <c r="A4" s="12">
         <v>1</v>
       </c>
+      <c r="B4" s="11" t="s">
+        <v>99</v>
+      </c>
       <c r="C4" s="11" t="s">
         <v>40</v>
       </c>
@@ -1253,6 +1271,9 @@
       <c r="A5" s="12">
         <v>2</v>
       </c>
+      <c r="B5" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="C5" s="8" t="s">
         <v>39</v>
       </c>
@@ -1271,6 +1292,9 @@
       <c r="A6" s="12">
         <v>3</v>
       </c>
+      <c r="B6" s="11" t="s">
+        <v>100</v>
+      </c>
       <c r="C6" s="11" t="s">
         <v>30</v>
       </c>
@@ -1288,6 +1312,9 @@
       <c r="A7" s="12">
         <v>4</v>
       </c>
+      <c r="B7" s="11" t="s">
+        <v>101</v>
+      </c>
       <c r="C7" s="11" t="s">
         <v>31</v>
       </c>
@@ -1304,6 +1331,9 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>5</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>32</v>

</xml_diff>